<commit_message>
Novas alterações com alura
</commit_message>
<xml_diff>
--- a/materiais/acidentes/Condiçao Meteorológica.xlsx
+++ b/materiais/acidentes/Condiçao Meteorológica.xlsx
@@ -22,37 +22,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t xml:space="preserve">condicao_metereologica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chuva               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Céu Claro           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garoa/Chuvisco      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granizo             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignorado            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neve                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nevoeiro/Neblina    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nublado             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sol                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vento               </t>
+    <t xml:space="preserve">Céu Claro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chuva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garoa/Chuvisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granizo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignorado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nevoeiro/Neblina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nublado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vento</t>
   </si>
 </sst>
 </file>
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,13 +83,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,12 +127,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,7 +152,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -173,7 +162,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>